<commit_message>
depuración - Módulo de video terminado
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
   <si>
     <t>TÍTULO</t>
   </si>
@@ -110,7 +110,7 @@
     <t>Gratis</t>
   </si>
   <si>
-    <t>2019</t>
+    <t>2020</t>
   </si>
   <si>
     <t>Temporada 02</t>
@@ -119,7 +119,7 @@
     <t>Temporada 01</t>
   </si>
   <si>
-    <t>5</t>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -481,7 +481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -633,6 +633,46 @@
         <v>24</v>
       </c>
     </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2016</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -640,7 +680,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -734,13 +774,36 @@
       <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
+      <c r="F4" s="1">
+        <v>2019</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
uso eficaz de pipes entre funciones y GUI
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
   <si>
     <t>TÍTULO</t>
   </si>
@@ -89,6 +89,9 @@
     <t>HD</t>
   </si>
   <si>
+    <t>2019</t>
+  </si>
+  <si>
     <t>$3.490</t>
   </si>
   <si>
@@ -110,16 +113,10 @@
     <t>Gratis</t>
   </si>
   <si>
-    <t>2020</t>
-  </si>
-  <si>
     <t>Temporada 02</t>
   </si>
   <si>
     <t>Temporada 01</t>
-  </si>
-  <si>
-    <t>1</t>
   </si>
 </sst>
 </file>
@@ -481,7 +478,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -590,7 +587,7 @@
         <v>2017</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -610,7 +607,7 @@
         <v>2019</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -630,7 +627,7 @@
         <v>2019</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -650,7 +647,7 @@
         <v>2019</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -671,6 +668,86 @@
       </c>
       <c r="F9" s="1">
         <v>2016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -680,7 +757,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -709,18 +786,18 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -740,10 +817,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>21</v>
@@ -763,10 +840,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -786,10 +863,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -797,14 +874,37 @@
       <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>31</v>
+      <c r="F5" s="1">
+        <v>2020</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>34</v>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalización módulo de herramienta de software
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="35">
   <si>
     <t>TÍTULO</t>
   </si>
@@ -89,9 +89,6 @@
     <t>HD</t>
   </si>
   <si>
-    <t>2019</t>
-  </si>
-  <si>
     <t>$3.490</t>
   </si>
   <si>
@@ -113,10 +110,16 @@
     <t>Gratis</t>
   </si>
   <si>
+    <t>2020</t>
+  </si>
+  <si>
     <t>Temporada 02</t>
   </si>
   <si>
     <t>Temporada 01</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -478,7 +481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -587,7 +590,7 @@
         <v>2017</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -607,7 +610,7 @@
         <v>2019</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -627,7 +630,7 @@
         <v>2019</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -647,7 +650,7 @@
         <v>2019</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -687,7 +690,7 @@
         <v>2019</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -746,7 +749,47 @@
       <c r="E13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -757,7 +800,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -786,18 +829,18 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -817,10 +860,10 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>21</v>
@@ -840,10 +883,10 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -863,10 +906,10 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -886,10 +929,10 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -905,6 +948,29 @@
       </c>
       <c r="H6" s="1">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
perfeccionamiento buttons y widgets
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>TÍTULO</t>
   </si>
@@ -41,18 +41,39 @@
     <t>Guerrilla del Oro</t>
   </si>
   <si>
+    <t>Planeta Hostil</t>
+  </si>
+  <si>
+    <t>Sumergidos</t>
+  </si>
+  <si>
     <t>NATIONAL GEOGRAPHIC</t>
   </si>
   <si>
+    <t>WILD</t>
+  </si>
+  <si>
     <t>Premium</t>
   </si>
   <si>
+    <t>Arriendo</t>
+  </si>
+  <si>
     <t>Documental</t>
   </si>
   <si>
+    <t>Acción</t>
+  </si>
+  <si>
     <t>HD</t>
   </si>
   <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>$3.490</t>
+  </si>
+  <si>
     <t>TEMPORADAS</t>
   </si>
   <si>
@@ -62,19 +83,19 @@
     <t>My Brilliant Friend</t>
   </si>
   <si>
+    <t>The Outsider - El Visitante</t>
+  </si>
+  <si>
     <t>Gratis</t>
   </si>
   <si>
     <t>Drama</t>
   </si>
   <si>
-    <t>2020</t>
-  </si>
-  <si>
     <t>Temporada 02</t>
   </si>
   <si>
-    <t>1</t>
+    <t>Temporada 01</t>
   </si>
 </sst>
 </file>
@@ -436,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -473,19 +494,59 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -495,7 +556,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -524,33 +585,56 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>19</v>
+      <c r="F3" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
evolución interfaz y disegno
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>TÍTULO</t>
   </si>
@@ -38,18 +38,12 @@
     <t>PRECIO</t>
   </si>
   <si>
-    <t>Guerrilla del Oro</t>
-  </si>
-  <si>
     <t>Planeta Hostil</t>
   </si>
   <si>
     <t>Sumergidos</t>
   </si>
   <si>
-    <t>NATIONAL GEOGRAPHIC</t>
-  </si>
-  <si>
     <t>WILD</t>
   </si>
   <si>
@@ -80,19 +74,10 @@
     <t>EPISODIOS</t>
   </si>
   <si>
-    <t>My Brilliant Friend</t>
-  </si>
-  <si>
     <t>The Outsider - El Visitante</t>
   </si>
   <si>
     <t>Gratis</t>
-  </si>
-  <si>
-    <t>Drama</t>
-  </si>
-  <si>
-    <t>Temporada 02</t>
   </si>
   <si>
     <t>Temporada 01</t>
@@ -457,7 +442,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -494,16 +479,16 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="1">
         <v>2019</v>
@@ -513,40 +498,20 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -556,7 +521,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -585,55 +550,32 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="1">
         <v>2020</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H2" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1">
-        <v>2020</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="1">
         <v>10</v>
       </c>
     </row>

</xml_diff>